<commit_message>
Modificações Tratamento de Erros
</commit_message>
<xml_diff>
--- a/Main/bin/Debug/TabelaShiftReduce.xlsx
+++ b/Main/bin/Debug/TabelaShiftReduce.xlsx
@@ -323,9 +323,6 @@
     <t>E9</t>
   </si>
   <si>
-    <t>E14</t>
-  </si>
-  <si>
     <t>E15</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
     <t>E13</t>
   </si>
   <si>
-    <t>E10</t>
-  </si>
-  <si>
     <t>E16</t>
   </si>
   <si>
@@ -360,6 +354,12 @@
   </si>
   <si>
     <t>E19</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>E21</t>
   </si>
 </sst>
 </file>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -834,10 +834,10 @@
         <v>11</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>91</v>
@@ -1124,28 +1124,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>33</v>
@@ -1154,40 +1154,40 @@
         <v>34</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Z5" s="2">
         <v>5</v>
@@ -1210,70 +1210,70 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AA6" s="2">
         <v>23</v>
@@ -1358,28 +1358,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>33</v>
@@ -1388,40 +1388,40 @@
         <v>34</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Z8" s="2">
         <v>15</v>
@@ -1444,28 +1444,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>33</v>
@@ -1474,40 +1474,40 @@
         <v>34</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="V9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Z9" s="2">
         <v>46</v>
@@ -1530,28 +1530,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>33</v>
@@ -1560,40 +1560,40 @@
         <v>34</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="V10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="W10" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Z10" s="2">
         <v>47</v>
@@ -1684,70 +1684,70 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="W12" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:38" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1897,28 +1897,28 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>42</v>
@@ -1927,40 +1927,40 @@
         <v>34</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AD15" s="2">
         <v>19</v>
@@ -2196,34 +2196,34 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>48</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>49</v>
@@ -2232,34 +2232,34 @@
         <v>50</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="T19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="U19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="V19" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AE19" s="2">
         <v>33</v>
@@ -2341,28 +2341,28 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>33</v>
@@ -2371,40 +2371,40 @@
         <v>34</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>44</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="W21" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AD21" s="2">
         <v>19</v>
@@ -2427,28 +2427,28 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>42</v>
@@ -2457,40 +2457,40 @@
         <v>34</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U22" s="3" t="s">
         <v>44</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="W22" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AD22" s="2">
         <v>19</v>
@@ -2513,28 +2513,28 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>42</v>
@@ -2543,40 +2543,40 @@
         <v>34</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U23" s="3" t="s">
         <v>44</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AD23" s="2">
         <v>19</v>
@@ -2741,70 +2741,70 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="W26" s="7" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AA26" s="2">
         <v>51</v>
@@ -2960,19 +2960,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>57</v>
@@ -2984,46 +2984,46 @@
         <v>59</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC29" s="2">
         <v>28</v>
@@ -3673,70 +3673,70 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="M39" s="10" t="s">
         <v>71</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Q39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="R39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="S39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="T39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="U39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="V39" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="W39" s="7" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="AG39" s="2">
         <v>39</v>
@@ -3750,70 +3750,70 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="M40" s="10" t="s">
         <v>71</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="P40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Q40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="R40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="S40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="T40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="U40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="V40" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="W40" s="7" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="AH40" s="2">
         <v>53</v>
@@ -3898,70 +3898,70 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>92</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O42" s="10" t="s">
         <v>73</v>
       </c>
       <c r="P42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="S42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="T42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="U42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="V42" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="W42" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:37" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4111,70 +4111,70 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="M45" s="10" t="s">
         <v>71</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="P45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Q45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="R45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="S45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="T45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="U45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="V45" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="W45" s="7" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="AH45" s="2">
         <v>45</v>
@@ -4753,70 +4753,70 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R54" s="10" t="s">
         <v>83</v>
       </c>
       <c r="S54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W54" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:38" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4824,70 +4824,70 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T55" s="10" t="s">
         <v>84</v>
       </c>
       <c r="U55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V55" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W55" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:38" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4895,70 +4895,70 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S56" s="10" t="s">
         <v>85</v>
       </c>
       <c r="T56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="V56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W56" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:38" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4966,70 +4966,70 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="M57" s="10" t="s">
         <v>71</v>
       </c>
       <c r="N57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="O57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="P57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Q57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="R57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="S57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="T57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="U57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="V57" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="W57" s="7" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="AH57" s="2">
         <v>57</v>

</xml_diff>